<commit_message>
feat: replace html2image with Playwright for PNG export
html2image had viewport clipping issues with CSS max-width constraining
content to fixed viewport. Playwright's full_page=True screenshot captures
the entire timeline grid (07:00-22:00) with no clipping.

- Swap html2image → playwright sync API with headless Chromium
- Dynamic viewport width based on TIME_SLOTS count
- Write HTML to temp file, screenshot with full_page=True
- Update planning docs (EPCC_CODE, EPCC_PLAN, features, progress)

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/sample staff schedule.xlsx
+++ b/data/sample staff schedule.xlsx
@@ -58,36 +58,33 @@
     <t xml:space="preserve">7.00 am to 15.00 pm</t>
   </si>
   <si>
-    <t xml:space="preserve">Melany Vivar Tranquilo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olasunkanmi Akinmuyipitan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raquel Eusébio</t>
+    <t xml:space="preserve">King Alale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roksalana </t>
   </si>
   <si>
     <t xml:space="preserve">Shinde Gaikwad</t>
   </si>
   <si>
+    <t>Swahna</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shivahari Giri</t>
   </si>
   <si>
     <t xml:space="preserve">Jithin Reghuvaran</t>
   </si>
   <si>
-    <t xml:space="preserve">King Alale</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nyima Tashi</t>
   </si>
   <si>
+    <t xml:space="preserve">15.00 pm to 23.00 pm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eric Uwanikone</t>
   </si>
   <si>
-    <t xml:space="preserve">15.00 pm to 23.00 pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">Daniela Natasa Rostas</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Akanimo Desmond Ekpo</t>
+  </si>
+  <si>
+    <t>Raquel</t>
   </si>
 </sst>
 </file>
@@ -150,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
       <alignment horizontal="center" vertical="top"/>
@@ -159,6 +159,9 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -686,7 +689,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -780,7 +783,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -887,8 +890,8 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -913,8 +916,8 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -937,7 +940,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -963,10 +966,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -991,23 +994,23 @@
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
+      <c r="B12" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
         <v>9</v>
@@ -1015,7 +1018,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -1041,7 +1044,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1067,7 +1070,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -1085,36 +1088,44 @@
         <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" t="s">
-        <v>9</v>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>